<commit_message>
first commit add/delete/edit program file
</commit_message>
<xml_diff>
--- a/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
+++ b/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\eclipse-workspace-new\LMS_seleniumPhase2\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmman\git\Team7_TechTesters_selenium\LMS_seleniumPhase2\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE0170-65A4-4DEB-8EBB-370102782F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40864E44-A285-4B5E-80E3-20ED561DAFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="570" windowWidth="15375" windowHeight="9270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="3" r:id="rId1"/>
     <sheet name="BatchSheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Program" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -148,6 +149,18 @@
   </si>
   <si>
     <t>UIHackathon@02</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>programDesc</t>
+  </si>
+  <si>
+    <t>Team7LMS</t>
+  </si>
+  <si>
+    <t>Team7LMS18</t>
   </si>
 </sst>
 </file>
@@ -1019,17 +1032,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7CAC2F-0F82-4289-AA66-82910A557688}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1037,7 +1050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1058,27 +1071,27 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1142,7 +1155,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1171,7 +1184,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1200,7 +1213,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1220,7 +1233,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1284,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1313,7 +1326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1342,7 +1355,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1374,7 +1387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1432,7 +1445,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1461,7 +1474,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1494,4 +1507,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DF07DF-945C-4A22-ADAB-88F0C773E39F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
batch Edit integration changes commits
</commit_message>
<xml_diff>
--- a/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
+++ b/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\git\Team7_TechTesters_selenium\LMS_seleniumPhase2\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\git\Team7_TechTesters_selenium\Team7_integration\Team7_TechTesters_selenium\LMS_seleniumPhase2\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C216E11-C799-4CBC-A9E2-540FDA72F7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292FFB70-E2E6-4CC2-B0D5-FD1B64890540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>Active</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Batch Desc is mandatory</t>
   </si>
   <si>
-    <t>Empty BatchNoOfclasses</t>
-  </si>
-  <si>
-    <t>InActive</t>
-  </si>
-  <si>
     <t>UI Testing 1@@</t>
   </si>
   <si>
@@ -107,12 +101,6 @@
     <t>Batchclasses allows more digits</t>
   </si>
   <si>
-    <t>Batchstatus is null</t>
-  </si>
-  <si>
-    <t>BatchStatus is Inactive</t>
-  </si>
-  <si>
     <t>#4</t>
   </si>
   <si>
@@ -128,9 +116,6 @@
     <t>Team7-TechTesters-SDET-SDET01-0103</t>
   </si>
   <si>
-    <t>Team7-TechTesters@#-SDET-SDET01-0123</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -140,10 +125,10 @@
     <t>cancel</t>
   </si>
   <si>
-    <t>Team7-TechTesters-SDET-SDET01-0126</t>
-  </si>
-  <si>
-    <t>team7-techtesters-SDET-SDET01-0126</t>
+    <t>Team7-TechTesters@#-SDET-SDET01-01123</t>
+  </si>
+  <si>
+    <t>Team7-TechTesters-SDET-SDET01-09</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G1"/>
     </row>
@@ -1108,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1">
         <v>7</v>
@@ -1120,15 +1105,12 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>7</v>
@@ -1137,132 +1119,138 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>4</v>
+        <v>12345678901</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>12345678</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -1271,10 +1259,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1282,102 +1270,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1">
-        <v>12345678901</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1">
-        <v>12345678</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
         <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{F8C43735-C579-4BF3-AABB-6DE769E134DB}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{F8C43735-C579-4BF3-AABB-6DE769E134DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Integration with Delete Batch
</commit_message>
<xml_diff>
--- a/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
+++ b/LMS_seleniumPhase2/src/test/resources/TestData/LMSTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\git\Team7_TechTesters_selenium\Team7_integration\Team7_TechTesters_selenium\LMS_seleniumPhase2\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292FFB70-E2E6-4CC2-B0D5-FD1B64890540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DECBF1-9DF2-4212-9A65-87ED9DE9EF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
     <t>Team7-TechTesters@#-SDET-SDET01-01123</t>
   </si>
   <si>
-    <t>Team7-TechTesters-SDET-SDET01-09</t>
+    <t>Team7-TechTesters-SDET-SDET01-11</t>
   </si>
 </sst>
 </file>

</xml_diff>